<commit_message>
split documentation to have API specific section. Clarified Allergies
</commit_message>
<xml_diff>
--- a/docs/ObservationTypeTOVsLoincCode.xlsx
+++ b/docs/ObservationTypeTOVsLoincCode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.15-beta</t>
+    <t>0.1.16-beta</t>
   </si>
   <si>
     <t>Name</t>
@@ -398,10 +398,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>

</xml_diff>

<commit_message>
changing to be more formal now that it is VA github repo
</commit_message>
<xml_diff>
--- a/docs/ObservationTypeTOVsLoincCode.xlsx
+++ b/docs/ObservationTypeTOVsLoincCode.xlsx
@@ -24,13 +24,13 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://johnmoehrke.github.io/MHV-PHR/ConceptMap/ObservationTypeTOVsLoincCode</t>
+    <t>https://department-of-veterans-affairs.github.io/mhv-fhir-phr-mapping/ConceptMap/ObservationTypeTOVsLoincCode</t>
   </si>
   <si>
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.20-beta</t>
+    <t>0.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -66,7 +66,7 @@
     <t>Publisher</t>
   </si>
   <si>
-    <t>John Moehrke (himself)</t>
+    <t>VA Digital Services</t>
   </si>
   <si>
     <t>Contact</t>

</xml_diff>

<commit_message>
not using meta.lastUpdated for any mapping as HAPI overwrites it Organization, Location, and Practitioner will always be contained add old maps for allergies and immunizations better distinction of mhv-fhir-phr vs MHV-PHR in names of things Vitals, fixes in Vitals, Vitals codes add VUID concept maps from KBS advise Vitals.code.coding as a VUID if 7 digits Vitals.component, leave this to us-core Vitals removed sample xslt as it was badly out of date Allergies.recorder.display should be populated Change Notes for PN to Progress Notes from KBS advise Immunization.location use contained resource
</commit_message>
<xml_diff>
--- a/docs/ObservationTypeTOVsLoincCode.xlsx
+++ b/docs/ObservationTypeTOVsLoincCode.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="108">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-03-29</t>
+    <t>2023-08-25</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -84,7 +84,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Map between VitalSignTO.type(ObservationTypeTO.name) string and LOINC code.</t>
+    <t>Map between VitalSignTO.type(ObservationTypeTO.name) VUID/string and LOINC code.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -108,7 +108,7 @@
     <t>Target</t>
   </si>
   <si>
-    <t>http://service.via.med.va.gov/ObservationTypeTO</t>
+    <t>urn:oid:2.16.840.1.113883.6.233</t>
   </si>
   <si>
     <t/>
@@ -117,6 +117,9 @@
     <t>http://loinc.org</t>
   </si>
   <si>
+    <t>unknown</t>
+  </si>
+  <si>
     <t>ABDMONAL GIRTH</t>
   </si>
   <si>
@@ -129,16 +132,19 @@
     <t>Abdominal circumference</t>
   </si>
   <si>
+    <t>4688718</t>
+  </si>
+  <si>
     <t>AUDIOMETRY</t>
   </si>
   <si>
-    <t>source-is-narrower-than-target</t>
-  </si>
-  <si>
-    <t>89015-2</t>
-  </si>
-  <si>
-    <t>Pure tone threshold audiometry panel</t>
+    <t>28615-3</t>
+  </si>
+  <si>
+    <t>Audiology study</t>
+  </si>
+  <si>
+    <t>4500634</t>
   </si>
   <si>
     <t>BLOOD PRESSURE</t>
@@ -150,6 +156,9 @@
     <t>Blood pressure panel with all children optional</t>
   </si>
   <si>
+    <t>4500638</t>
+  </si>
+  <si>
     <t>TEMPERATURE</t>
   </si>
   <si>
@@ -159,6 +168,9 @@
     <t>Body temperature</t>
   </si>
   <si>
+    <t>4688719</t>
+  </si>
+  <si>
     <t>CENTRAL VENOUS PRESSURE</t>
   </si>
   <si>
@@ -168,25 +180,31 @@
     <t>Central venous pressure (CVP) Mean</t>
   </si>
   <si>
+    <t>4688720</t>
+  </si>
+  <si>
     <t>CIRCUMFERENCE%2FGIRTH</t>
   </si>
   <si>
-    <t>56086-2</t>
-  </si>
-  <si>
-    <t>Adult Waist Circumference Protocol</t>
+    <t>9844-2</t>
+  </si>
+  <si>
+    <t>Body region Circumference</t>
+  </si>
+  <si>
+    <t>4688721</t>
   </si>
   <si>
     <t>FETAL HEART TONES</t>
   </si>
   <si>
-    <t>related-to</t>
-  </si>
-  <si>
-    <t>55283-6</t>
-  </si>
-  <si>
-    <t>Fetal Heart rate</t>
+    <t>11616-0</t>
+  </si>
+  <si>
+    <t>Fetal Heart Narrative Activity US</t>
+  </si>
+  <si>
+    <t>4688722</t>
   </si>
   <si>
     <t>FUNDAL HEIGHT</t>
@@ -198,7 +216,7 @@
     <t>Uterus Fundal height Tape measure</t>
   </si>
   <si>
-    <t>HEADCIRCUMFERENCE</t>
+    <t>HEAD CIRCUMFERENCE</t>
   </si>
   <si>
     <t>9843-4</t>
@@ -207,13 +225,19 @@
     <t>Head Occipital-frontal circumference</t>
   </si>
   <si>
+    <t>4688723</t>
+  </si>
+  <si>
     <t>HEARING</t>
   </si>
   <si>
-    <t>58232-0</t>
-  </si>
-  <si>
-    <t>Hearing loss risk indicators [Identifier]</t>
+    <t>32437-6</t>
+  </si>
+  <si>
+    <t>Physical findings of Hearing</t>
+  </si>
+  <si>
+    <t>4688724</t>
   </si>
   <si>
     <t>HEIGHT</t>
@@ -225,6 +249,9 @@
     <t>Body height</t>
   </si>
   <si>
+    <t>4500635</t>
+  </si>
+  <si>
     <t>PAIN</t>
   </si>
   <si>
@@ -234,6 +261,9 @@
     <t>Pain severity - 0-10 verbal numeric rating [Score] - Reported</t>
   </si>
   <si>
+    <t>4500637</t>
+  </si>
+  <si>
     <t>PULSE OXIMETRY</t>
   </si>
   <si>
@@ -243,6 +273,9 @@
     <t>Oxygen saturation in Arterial blood</t>
   </si>
   <si>
+    <t>4500636</t>
+  </si>
+  <si>
     <t>PULSE</t>
   </si>
   <si>
@@ -252,6 +285,9 @@
     <t>Heart rate</t>
   </si>
   <si>
+    <t>4688725</t>
+  </si>
+  <si>
     <t>RESPIRATION</t>
   </si>
   <si>
@@ -261,13 +297,37 @@
     <t>Respiratory Rate</t>
   </si>
   <si>
+    <t>4688726</t>
+  </si>
+  <si>
     <t>TONOMETRY</t>
   </si>
   <si>
-    <t>LP76227-5</t>
-  </si>
-  <si>
-    <t>Tonometry</t>
+    <t>28630-2</t>
+  </si>
+  <si>
+    <t>Tonometry study</t>
+  </si>
+  <si>
+    <t>4688727</t>
+  </si>
+  <si>
+    <t>VISION CORRECTED</t>
+  </si>
+  <si>
+    <t>70936-0</t>
+  </si>
+  <si>
+    <t>Vision testing Narrative</t>
+  </si>
+  <si>
+    <t>4688728</t>
+  </si>
+  <si>
+    <t>VISION UNCORRECTED</t>
+  </si>
+  <si>
+    <t>4500639</t>
   </si>
   <si>
     <t>WEIGHT</t>
@@ -545,7 +605,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -589,255 +649,323 @@
       <c r="A3" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" t="s" s="2">
+        <v>35</v>
+      </c>
       <c r="C3" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="B4" t="s" s="2">
+        <v>40</v>
+      </c>
       <c r="C4" t="s" s="2">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="B5" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="C5" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="B6" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="B6" t="s" s="2">
+        <v>48</v>
+      </c>
       <c r="C6" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s" s="2">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>52</v>
+      </c>
       <c r="C7" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s" s="2">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="B8" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="B8" t="s" s="2">
+        <v>56</v>
+      </c>
       <c r="C8" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s" s="2">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="B9" t="s" s="2">
+        <v>60</v>
+      </c>
       <c r="C9" t="s" s="2">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s" s="2">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="B10" t="s" s="2">
+        <v>64</v>
+      </c>
       <c r="C10" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="B11" t="s" s="2">
+        <v>67</v>
+      </c>
       <c r="C11" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s" s="2">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>71</v>
+      </c>
       <c r="C12" t="s" s="2">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s" s="2">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>75</v>
+      </c>
       <c r="C13" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s" s="2">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>79</v>
+      </c>
       <c r="C14" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s" s="2">
-        <v>72</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>83</v>
+      </c>
       <c r="C15" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s" s="2">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>87</v>
+      </c>
       <c r="C16" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s" s="2">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="B17" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="B17" t="s" s="2">
+        <v>91</v>
+      </c>
       <c r="C17" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="E17" t="s" s="2">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>95</v>
+      </c>
       <c r="C18" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s" s="2">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>85</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>99</v>
+      </c>
       <c r="C19" t="s" s="2">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s" s="2">
-        <v>87</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="B20" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="E20" t="s" s="2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="B21" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="E21" t="s" s="2">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>